<commit_message>
3x speed up for 4 threads
</commit_message>
<xml_diff>
--- a/ChunkingTest.xlsx
+++ b/ChunkingTest.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Chunksize </t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Col. ONLY</t>
+  </si>
+  <si>
+    <t>N/A (split row and col)</t>
+  </si>
+  <si>
+    <t>Threads</t>
   </si>
 </sst>
 </file>
@@ -371,115 +377,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>5</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>30</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>754466</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>641386</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>608614</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>630682</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>1798856</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>1643520</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>1604400</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>1615570</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <f>B3/B2</f>
-        <v>2.3842770913467275</v>
       </c>
       <c r="C4" s="2">
         <f>C3/C2</f>
-        <v>2.5624506927185813</v>
+        <v>2.3842770913467275</v>
       </c>
       <c r="D4" s="2">
         <f>D3/D2</f>
-        <v>2.6361536211786123</v>
+        <v>2.5624506927185813</v>
       </c>
       <c r="E4" s="2">
         <f>E3/E2</f>
+        <v>2.6361536211786123</v>
+      </c>
+      <c r="F4" s="2">
+        <f>F3/F2</f>
         <v>2.5616237660183736</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C7" s="3">
         <v>1937770</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>1949490</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8" s="1">
         <v>433956</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3">
+      <c r="C9" s="3">
         <v>1469920</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
+        <v>670978</v>
+      </c>
+      <c r="C13" s="1">
+        <v>809590</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1030280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="3">
+        <v>1937770</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1937770</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1937770</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="2">
+        <f>B14/B13</f>
+        <v>2.8879784434064901</v>
+      </c>
+      <c r="C15" s="2">
+        <f>C14/C13</f>
+        <v>2.393520176879655</v>
+      </c>
+      <c r="D15" s="2">
+        <f>D14/D13</f>
+        <v>1.8808188065380285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>